<commit_message>
Cambio la Fig. de Barras y reubico la Cita del Abstract
</commit_message>
<xml_diff>
--- a/Rcode/barrasRcode/areaTiempo.xlsx
+++ b/Rcode/barrasRcode/areaTiempo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">NoncombinationalArea</t>
   </si>
   <si>
-    <t xml:space="preserve">Impl1</t>
+    <t xml:space="preserve">impl1</t>
   </si>
   <si>
     <t xml:space="preserve">impl2</t>
@@ -43,10 +43,7 @@
     <t xml:space="preserve">impl3</t>
   </si>
   <si>
-    <t xml:space="preserve">impl4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Impl5</t>
+    <t xml:space="preserve">Impl4</t>
   </si>
 </sst>
 </file>
@@ -175,19 +172,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="995" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="996" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="995" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="996" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -209,13 +206,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>-3.65</v>
+        <v>-0.76</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>291201.116637</v>
+        <v>294733.068172</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>58830.508095</v>
+        <v>62955.185703</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -223,13 +220,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>-0.76</v>
+        <v>-0.81</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>294733.068172</v>
+        <v>233949.801414</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>62955.185703</v>
+        <v>56229.647552</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -237,40 +234,26 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>-0.81</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>233949.801414</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>56229.647552</v>
+        <v>195877.841872</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>64463.04657</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="0" t="n">
         <v>195877.841872</v>
       </c>
-      <c r="D5" s="4" t="n">
-        <v>64463.04657</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>195877.841872</v>
-      </c>
-      <c r="D6" s="0" t="n">
+      <c r="D5" s="0" t="n">
         <v>64463.04657</v>
       </c>
     </row>

</xml_diff>